<commit_message>
nextstrain test build 5/12/21
</commit_message>
<xml_diff>
--- a/pre-analyses/extra_metadata.xlsx
+++ b/pre-analyses/extra_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rle29/Google_Drive_Yale/Git_Projects/ncov_AB/pre-analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4321FA-79AC-254C-8097-559DEC836E53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DC6BF3-1C7C-254A-8219-0F8B608FFDAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9040" yWindow="500" windowWidth="22080" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="500" windowWidth="22080" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample metadata" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8890" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9367" uniqueCount="1058">
   <si>
     <t>Sample-ID</t>
   </si>
@@ -3068,6 +3068,165 @@
   </si>
   <si>
     <t>2021-04-24</t>
+  </si>
+  <si>
+    <t>JAX001199</t>
+  </si>
+  <si>
+    <t>JAX001203</t>
+  </si>
+  <si>
+    <t>JAX001205</t>
+  </si>
+  <si>
+    <t>JAX001209</t>
+  </si>
+  <si>
+    <t>JAX001211</t>
+  </si>
+  <si>
+    <t>JAX001212</t>
+  </si>
+  <si>
+    <t>JAX001213</t>
+  </si>
+  <si>
+    <t>JAX001214</t>
+  </si>
+  <si>
+    <t>JAX001215</t>
+  </si>
+  <si>
+    <t>JAX001216</t>
+  </si>
+  <si>
+    <t>JAX001217</t>
+  </si>
+  <si>
+    <t>JAX001218</t>
+  </si>
+  <si>
+    <t>JAX001219</t>
+  </si>
+  <si>
+    <t>JAX001220</t>
+  </si>
+  <si>
+    <t>JAX001221</t>
+  </si>
+  <si>
+    <t>JAX001223</t>
+  </si>
+  <si>
+    <t>JAX001224</t>
+  </si>
+  <si>
+    <t>JAX001225</t>
+  </si>
+  <si>
+    <t>JAX001226</t>
+  </si>
+  <si>
+    <t>JAX001227</t>
+  </si>
+  <si>
+    <t>JAX001228</t>
+  </si>
+  <si>
+    <t>JAX001229</t>
+  </si>
+  <si>
+    <t>JAX001230</t>
+  </si>
+  <si>
+    <t>JAX001231</t>
+  </si>
+  <si>
+    <t>JAX001232</t>
+  </si>
+  <si>
+    <t>JAX001234</t>
+  </si>
+  <si>
+    <t>JAX001235</t>
+  </si>
+  <si>
+    <t>JAX001236</t>
+  </si>
+  <si>
+    <t>JAX001237</t>
+  </si>
+  <si>
+    <t>JAX001238</t>
+  </si>
+  <si>
+    <t>JAX001239</t>
+  </si>
+  <si>
+    <t>JAX001240</t>
+  </si>
+  <si>
+    <t>JAX001242</t>
+  </si>
+  <si>
+    <t>JAX001243</t>
+  </si>
+  <si>
+    <t>JAX001244</t>
+  </si>
+  <si>
+    <t>JAX001245</t>
+  </si>
+  <si>
+    <t>JAX001247</t>
+  </si>
+  <si>
+    <t>JAX001248</t>
+  </si>
+  <si>
+    <t>JAX001250</t>
+  </si>
+  <si>
+    <t>JAX001252</t>
+  </si>
+  <si>
+    <t>JAX001254</t>
+  </si>
+  <si>
+    <t>JAX001255</t>
+  </si>
+  <si>
+    <t>JAX001256</t>
+  </si>
+  <si>
+    <t>JAX001257</t>
+  </si>
+  <si>
+    <t>JAX001258</t>
+  </si>
+  <si>
+    <t>JAX001259</t>
+  </si>
+  <si>
+    <t>JAX001260</t>
+  </si>
+  <si>
+    <t>JAX001261</t>
+  </si>
+  <si>
+    <t>JAX001262</t>
+  </si>
+  <si>
+    <t>JAX001263</t>
+  </si>
+  <si>
+    <t>JAX001264</t>
+  </si>
+  <si>
+    <t>JAX001265</t>
+  </si>
+  <si>
+    <t>JAX001266</t>
   </si>
 </sst>
 </file>
@@ -3405,10 +3564,10 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B865" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B924" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K879" sqref="K879"/>
+      <selection pane="bottomRight" activeCell="G900" sqref="G900"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -34863,250 +35022,1893 @@
       </c>
     </row>
     <row r="899" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D899" s="10"/>
-      <c r="L899" s="10"/>
+      <c r="A899" s="14" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B899" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C899" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D899" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E899" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F899" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G899" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H899" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J899" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K899" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L899" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="900" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D900" s="10"/>
-      <c r="L900" s="10"/>
+      <c r="A900" s="14" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B900" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C900" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D900" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E900" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F900" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G900" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H900" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J900" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K900" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L900" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="901" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D901" s="10"/>
-      <c r="L901" s="10"/>
+      <c r="A901" s="14" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B901" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C901" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D901" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E901" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F901" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G901" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H901" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J901" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K901" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L901" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="902" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D902" s="10"/>
-      <c r="L902" s="10"/>
+      <c r="A902" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B902" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C902" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D902" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E902" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F902" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G902" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H902" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J902" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K902" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L902" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="903" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D903" s="10"/>
-      <c r="L903" s="10"/>
+      <c r="A903" s="14" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B903" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C903" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D903" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E903" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F903" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G903" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H903" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J903" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K903" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L903" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="904" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D904" s="10"/>
-      <c r="L904" s="10"/>
+      <c r="A904" s="14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B904" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C904" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D904" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E904" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F904" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G904" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H904" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J904" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K904" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L904" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="905" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D905" s="10"/>
-      <c r="L905" s="10"/>
+      <c r="A905" s="14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B905" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C905" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D905" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E905" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F905" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G905" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H905" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J905" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K905" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L905" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="906" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D906" s="10"/>
-      <c r="L906" s="10"/>
+      <c r="A906" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B906" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C906" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D906" s="11">
+        <v>44315</v>
+      </c>
+      <c r="E906" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F906" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G906" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H906" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J906" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K906" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L906" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="907" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D907" s="10"/>
-      <c r="L907" s="10"/>
+      <c r="A907" s="14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B907" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C907" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D907" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E907" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F907" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G907" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H907" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J907" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K907" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L907" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="908" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D908" s="10"/>
-      <c r="L908" s="10"/>
+      <c r="A908" s="14" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B908" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C908" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D908" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E908" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F908" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G908" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H908" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J908" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K908" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L908" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="909" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D909" s="10"/>
-      <c r="L909" s="10"/>
+      <c r="A909" s="14" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B909" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C909" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D909" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E909" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F909" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G909" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H909" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J909" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K909" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L909" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="910" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D910" s="10"/>
-      <c r="L910" s="10"/>
+      <c r="A910" s="14" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B910" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C910" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D910" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E910" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F910" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G910" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H910" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J910" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K910" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L910" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="911" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D911" s="10"/>
-      <c r="L911" s="10"/>
+      <c r="A911" s="14" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B911" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C911" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D911" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E911" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F911" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G911" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H911" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J911" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K911" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L911" s="10">
+        <v>44327</v>
+      </c>
     </row>
     <row r="912" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D912" s="10"/>
-      <c r="L912" s="10"/>
-    </row>
-    <row r="913" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D913" s="10"/>
-      <c r="L913" s="10"/>
-    </row>
-    <row r="914" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D914" s="10"/>
-      <c r="L914" s="10"/>
-    </row>
-    <row r="915" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D915" s="10"/>
-      <c r="L915" s="10"/>
-    </row>
-    <row r="916" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D916" s="10"/>
-      <c r="L916" s="10"/>
-    </row>
-    <row r="917" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D917" s="10"/>
-      <c r="L917" s="10"/>
-    </row>
-    <row r="918" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D918" s="10"/>
-      <c r="L918" s="10"/>
-    </row>
-    <row r="919" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D919" s="10"/>
-      <c r="L919" s="10"/>
-    </row>
-    <row r="920" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D920" s="10"/>
-      <c r="L920" s="10"/>
-    </row>
-    <row r="921" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D921" s="10"/>
-      <c r="L921" s="10"/>
-    </row>
-    <row r="922" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D922" s="10"/>
-      <c r="L922" s="10"/>
-    </row>
-    <row r="923" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D923" s="10"/>
-      <c r="L923" s="10"/>
-    </row>
-    <row r="924" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D924" s="10"/>
-      <c r="L924" s="10"/>
-    </row>
-    <row r="925" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D925" s="10"/>
-      <c r="L925" s="10"/>
-    </row>
-    <row r="926" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D926" s="10"/>
-      <c r="L926" s="10"/>
-    </row>
-    <row r="927" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D927" s="10"/>
-      <c r="L927" s="10"/>
-    </row>
-    <row r="928" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D928" s="10"/>
-      <c r="L928" s="10"/>
-    </row>
-    <row r="929" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D929" s="10"/>
-      <c r="L929" s="10"/>
-    </row>
-    <row r="930" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D930" s="10"/>
-      <c r="L930" s="10"/>
-    </row>
-    <row r="931" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D931" s="10"/>
-      <c r="L931" s="10"/>
-    </row>
-    <row r="932" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D932" s="10"/>
-      <c r="L932" s="10"/>
-    </row>
-    <row r="933" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D933" s="10"/>
-      <c r="L933" s="10"/>
-    </row>
-    <row r="934" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D934" s="10"/>
-      <c r="L934" s="10"/>
-    </row>
-    <row r="935" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D935" s="10"/>
-      <c r="L935" s="10"/>
-    </row>
-    <row r="936" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D936" s="10"/>
-      <c r="L936" s="10"/>
-    </row>
-    <row r="937" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D937" s="10"/>
-      <c r="L937" s="10"/>
-    </row>
-    <row r="938" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D938" s="10"/>
-      <c r="L938" s="10"/>
-    </row>
-    <row r="939" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D939" s="10"/>
-      <c r="L939" s="10"/>
-    </row>
-    <row r="940" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D940" s="10"/>
-      <c r="L940" s="10"/>
-    </row>
-    <row r="941" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D941" s="10"/>
-      <c r="L941" s="10"/>
-    </row>
-    <row r="942" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D942" s="10"/>
-      <c r="L942" s="10"/>
-    </row>
-    <row r="943" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D943" s="10"/>
-      <c r="L943" s="10"/>
-    </row>
-    <row r="944" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D944" s="10"/>
-      <c r="L944" s="10"/>
-    </row>
-    <row r="945" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D945" s="10"/>
-      <c r="L945" s="10"/>
-    </row>
-    <row r="946" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D946" s="10"/>
-      <c r="L946" s="10"/>
-    </row>
-    <row r="947" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D947" s="10"/>
-      <c r="L947" s="10"/>
-    </row>
-    <row r="948" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D948" s="10"/>
-      <c r="L948" s="10"/>
-    </row>
-    <row r="949" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D949" s="10"/>
-      <c r="L949" s="10"/>
-    </row>
-    <row r="950" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D950" s="10"/>
-      <c r="L950" s="10"/>
-    </row>
-    <row r="951" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D951" s="10"/>
-      <c r="L951" s="10"/>
-    </row>
-    <row r="952" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A912" s="14" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B912" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C912" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D912" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E912" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F912" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G912" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H912" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J912" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K912" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L912" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="913" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A913" s="14" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B913" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C913" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D913" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E913" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F913" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G913" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H913" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J913" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K913" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L913" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="914" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A914" s="14" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B914" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C914" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D914" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E914" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F914" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G914" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H914" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J914" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K914" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L914" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="915" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A915" s="14" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B915" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C915" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D915" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E915" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F915" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G915" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H915" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J915" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K915" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L915" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="916" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A916" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B916" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C916" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D916" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E916" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F916" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G916" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H916" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J916" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K916" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L916" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="917" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A917" s="14" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B917" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C917" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D917" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E917" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F917" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G917" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H917" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J917" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K917" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L917" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="918" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A918" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B918" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C918" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D918" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E918" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F918" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G918" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H918" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J918" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K918" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L918" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="919" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A919" s="14" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B919" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C919" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D919" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E919" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F919" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G919" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H919" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J919" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K919" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L919" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="920" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A920" s="14" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B920" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C920" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D920" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E920" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F920" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G920" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H920" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J920" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K920" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L920" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="921" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A921" s="14" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B921" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C921" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D921" s="11">
+        <v>44315</v>
+      </c>
+      <c r="E921" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F921" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G921" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H921" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J921" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K921" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L921" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="922" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A922" s="14" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B922" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C922" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D922" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E922" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F922" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G922" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H922" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J922" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K922" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L922" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="923" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A923" s="14" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B923" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C923" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D923" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E923" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F923" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G923" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H923" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J923" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K923" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L923" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="924" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A924" s="14" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B924" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C924" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D924" s="11">
+        <v>44316</v>
+      </c>
+      <c r="E924" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F924" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G924" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H924" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J924" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K924" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L924" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="925" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A925" s="14" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B925" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C925" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D925" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E925" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F925" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G925" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H925" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J925" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K925" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L925" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="926" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A926" s="14" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B926" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C926" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D926" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E926" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F926" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G926" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H926" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J926" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K926" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L926" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="927" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A927" s="14" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B927" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C927" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D927" s="11">
+        <v>44316</v>
+      </c>
+      <c r="E927" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F927" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G927" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H927" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J927" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K927" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L927" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="928" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A928" s="14" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B928" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C928" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D928" s="11">
+        <v>44315</v>
+      </c>
+      <c r="E928" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="F928" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G928" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H928" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J928" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K928" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L928" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="929" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A929" s="14" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B929" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C929" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D929" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E929" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F929" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G929" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H929" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J929" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K929" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L929" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="930" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A930" s="14" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B930" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C930" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D930" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E930" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F930" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G930" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H930" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J930" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K930" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L930" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="931" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A931" s="14" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B931" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C931" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D931" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E931" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F931" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G931" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H931" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J931" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K931" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L931" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="932" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A932" s="14" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B932" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C932" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D932" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E932" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F932" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G932" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H932" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J932" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K932" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L932" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="933" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A933" s="14" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B933" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C933" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D933" s="11">
+        <v>44317</v>
+      </c>
+      <c r="E933" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F933" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G933" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H933" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J933" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K933" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L933" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="934" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A934" s="14" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B934" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C934" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D934" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E934" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F934" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G934" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H934" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J934" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K934" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L934" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="935" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A935" s="14" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B935" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C935" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D935" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E935" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F935" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G935" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H935" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J935" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K935" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L935" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="936" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A936" s="14" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B936" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C936" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D936" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E936" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F936" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G936" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H936" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J936" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K936" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L936" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="937" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A937" s="14" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B937" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C937" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D937" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E937" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F937" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G937" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H937" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J937" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K937" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L937" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="938" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A938" s="14" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B938" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C938" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D938" s="11">
+        <v>44315</v>
+      </c>
+      <c r="E938" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F938" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G938" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H938" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J938" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K938" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L938" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="939" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A939" s="14" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B939" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C939" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D939" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E939" s="15" t="s">
+        <v>631</v>
+      </c>
+      <c r="F939" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G939" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H939" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J939" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K939" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L939" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="940" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A940" s="14" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B940" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C940" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D940" s="11">
+        <v>44313</v>
+      </c>
+      <c r="E940" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F940" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G940" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H940" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J940" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K940" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L940" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="941" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A941" s="14" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B941" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C941" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D941" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E941" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F941" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G941" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H941" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J941" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K941" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L941" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="942" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A942" s="14" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B942" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C942" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D942" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E942" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F942" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G942" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H942" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J942" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K942" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L942" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="943" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A943" s="14" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B943" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C943" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D943" s="11">
+        <v>44317</v>
+      </c>
+      <c r="E943" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F943" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G943" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H943" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J943" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K943" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L943" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="944" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A944" s="14" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B944" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C944" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D944" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E944" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F944" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G944" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H944" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J944" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K944" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L944" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="945" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A945" s="14" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B945" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C945" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D945" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E945" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F945" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G945" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H945" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J945" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K945" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L945" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="946" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A946" s="14" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B946" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C946" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D946" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E946" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F946" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G946" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H946" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J946" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K946" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L946" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="947" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A947" s="14" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B947" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C947" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D947" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E947" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F947" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G947" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H947" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J947" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K947" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L947" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="948" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A948" s="14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B948" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C948" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D948" s="11">
+        <v>44316</v>
+      </c>
+      <c r="E948" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F948" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G948" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H948" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J948" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K948" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L948" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="949" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A949" s="14" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B949" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C949" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D949" s="11">
+        <v>44315</v>
+      </c>
+      <c r="E949" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F949" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G949" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H949" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J949" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K949" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L949" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="950" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A950" s="14" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B950" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C950" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D950" s="11">
+        <v>44314</v>
+      </c>
+      <c r="E950" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F950" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G950" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H950" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J950" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K950" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L950" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="951" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A951" s="14" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B951" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C951" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D951" s="11">
+        <v>44312</v>
+      </c>
+      <c r="E951" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F951" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G951" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H951" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J951" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K951" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L951" s="10">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="952" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D952" s="10"/>
       <c r="L952" s="10"/>
     </row>
-    <row r="953" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="953" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D953" s="10"/>
       <c r="L953" s="10"/>
     </row>
-    <row r="954" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="954" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D954" s="10"/>
       <c r="L954" s="10"/>
     </row>
-    <row r="955" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="955" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D955" s="10"/>
       <c r="L955" s="10"/>
     </row>
-    <row r="956" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="956" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D956" s="10"/>
       <c r="L956" s="10"/>
     </row>
-    <row r="957" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="957" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D957" s="10"/>
       <c r="L957" s="10"/>
     </row>
-    <row r="958" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="958" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D958" s="10"/>
       <c r="L958" s="10"/>
     </row>
-    <row r="959" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="959" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D959" s="10"/>
       <c r="L959" s="10"/>
     </row>
-    <row r="960" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="960" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D960" s="10"/>
       <c r="L960" s="10"/>
     </row>

</xml_diff>